<commit_message>
added basic reading files incomplete yet
</commit_message>
<xml_diff>
--- a/WD_filter/build/app/intermediates/assets/debug/flutter_assets/assets/csvFiles/items.xlsx
+++ b/WD_filter/build/app/intermediates/assets/debug/flutter_assets/assets/csvFiles/items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t xml:space="preserve">img</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">rarity</t>
   </si>
   <si>
-    <t xml:space="preserve">filter</t>
+    <t xml:space="preserve">description</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">race</t>
   </si>
   <si>
+    <t xml:space="preserve">bis</t>
+  </si>
+  <si>
     <t xml:space="preserve">item1</t>
   </si>
   <si>
@@ -55,7 +58,7 @@
     <t xml:space="preserve">trooper,judge</t>
   </si>
   <si>
-    <t xml:space="preserve">dunetown</t>
+    <t xml:space="preserve">skirmish</t>
   </si>
   <si>
     <t xml:space="preserve">nanotechnology</t>
@@ -64,6 +67,9 @@
     <t xml:space="preserve">human</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
     <t xml:space="preserve">item2</t>
   </si>
   <si>
@@ -73,10 +79,13 @@
     <t xml:space="preserve">assassin,constructor,trooper</t>
   </si>
   <si>
-    <t xml:space="preserve">skirmish</t>
-  </si>
-  <si>
     <t xml:space="preserve">xenotronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulson grenade “Doom D3”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trooper,lord commander</t>
   </si>
 </sst>
 </file>
@@ -152,8 +161,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -174,86 +187,124 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>18</v>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>